<commit_message>
melhorias na análise de vendas da bibi
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -14,15 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ano</t>
   </si>
   <si>
-    <t>total_item</t>
-  </si>
-  <si>
-    <t>Evolucao (%)</t>
+    <t>Produtos</t>
+  </si>
+  <si>
+    <t>Serviços</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Serviços (%)</t>
+  </si>
+  <si>
+    <t>Produtos (%)</t>
+  </si>
+  <si>
+    <t>Evolução Serviços (%)</t>
+  </si>
+  <si>
+    <t>Evolução Produtos (%)</t>
+  </si>
+  <si>
+    <t>Evolução Total (%)</t>
+  </si>
+  <si>
+    <t>Qtd Produtos</t>
+  </si>
+  <si>
+    <t>Qtd Serviços</t>
+  </si>
+  <si>
+    <t>Total Itens</t>
   </si>
 </sst>
 </file>
@@ -380,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,90 +423,327 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>2018</v>
       </c>
       <c r="B2">
-        <v>700197.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>484712.74</v>
+      </c>
+      <c r="C2">
+        <v>234945</v>
+      </c>
+      <c r="D2">
+        <v>719657.74</v>
+      </c>
+      <c r="E2">
+        <v>32.64676900438811</v>
+      </c>
+      <c r="F2">
+        <v>67.3532309956119</v>
+      </c>
+      <c r="J2">
+        <v>1780</v>
+      </c>
+      <c r="K2">
+        <v>1351</v>
+      </c>
+      <c r="L2">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2019</v>
       </c>
       <c r="B3">
-        <v>1741717.08</v>
+        <v>1161517.53</v>
       </c>
       <c r="C3">
-        <v>148.746604046605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>635735.5600000001</v>
+      </c>
+      <c r="D3">
+        <v>1797253.09</v>
+      </c>
+      <c r="E3">
+        <v>35.37262300659057</v>
+      </c>
+      <c r="F3">
+        <v>64.62737699340943</v>
+      </c>
+      <c r="G3">
+        <v>170.5890995764967</v>
+      </c>
+      <c r="H3">
+        <v>139.6300806948049</v>
+      </c>
+      <c r="I3">
+        <v>149.7372000751357</v>
+      </c>
+      <c r="J3">
+        <v>19043</v>
+      </c>
+      <c r="K3">
+        <v>3095</v>
+      </c>
+      <c r="L3">
+        <v>22138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>2020</v>
       </c>
       <c r="B4">
-        <v>3313857.03</v>
+        <v>2259471.49</v>
       </c>
       <c r="C4">
-        <v>90.26379588583926</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>1114043</v>
+      </c>
+      <c r="D4">
+        <v>3373514.49</v>
+      </c>
+      <c r="E4">
+        <v>33.02321668699872</v>
+      </c>
+      <c r="F4">
+        <v>66.97678331300128</v>
+      </c>
+      <c r="G4">
+        <v>75.23685477024441</v>
+      </c>
+      <c r="H4">
+        <v>94.52754105226464</v>
+      </c>
+      <c r="I4">
+        <v>87.70391931834153</v>
+      </c>
+      <c r="J4">
+        <v>42777</v>
+      </c>
+      <c r="K4">
+        <v>4019</v>
+      </c>
+      <c r="L4">
+        <v>46796</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2021</v>
       </c>
       <c r="B5">
-        <v>6564496.12</v>
+        <v>5399571.25</v>
       </c>
       <c r="C5">
-        <v>98.09231540685992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>1275732.01</v>
+      </c>
+      <c r="D5">
+        <v>6675303.26</v>
+      </c>
+      <c r="E5">
+        <v>19.11122177241727</v>
+      </c>
+      <c r="F5">
+        <v>80.88877822758272</v>
+      </c>
+      <c r="G5">
+        <v>14.51371356401863</v>
+      </c>
+      <c r="H5">
+        <v>138.9749671061351</v>
+      </c>
+      <c r="I5">
+        <v>97.87385765756707</v>
+      </c>
+      <c r="J5">
+        <v>64210</v>
+      </c>
+      <c r="K5">
+        <v>3896</v>
+      </c>
+      <c r="L5">
+        <v>68106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>2022</v>
       </c>
       <c r="B6">
-        <v>7360567.04</v>
+        <v>6143248.8</v>
       </c>
       <c r="C6">
-        <v>12.12691584316148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>1358552.5</v>
+      </c>
+      <c r="D6">
+        <v>7501801.3</v>
+      </c>
+      <c r="E6">
+        <v>18.10968387019262</v>
+      </c>
+      <c r="F6">
+        <v>81.89031612980739</v>
+      </c>
+      <c r="G6">
+        <v>6.49199748464413</v>
+      </c>
+      <c r="H6">
+        <v>13.77290002423803</v>
+      </c>
+      <c r="I6">
+        <v>12.38143059286267</v>
+      </c>
+      <c r="J6">
+        <v>67109</v>
+      </c>
+      <c r="K6">
+        <v>3959</v>
+      </c>
+      <c r="L6">
+        <v>71068</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2023</v>
       </c>
       <c r="B7">
-        <v>6932834.57</v>
+        <v>5961894</v>
       </c>
       <c r="C7">
-        <v>-5.811134762791315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>1198106.18</v>
+      </c>
+      <c r="D7">
+        <v>7160000.18</v>
+      </c>
+      <c r="E7">
+        <v>16.73332611564264</v>
+      </c>
+      <c r="F7">
+        <v>83.26667388435737</v>
+      </c>
+      <c r="G7">
+        <v>-11.81009346344731</v>
+      </c>
+      <c r="H7">
+        <v>-2.952099221506377</v>
+      </c>
+      <c r="I7">
+        <v>-4.556253975961743</v>
+      </c>
+      <c r="J7">
+        <v>70506</v>
+      </c>
+      <c r="K7">
+        <v>3843</v>
+      </c>
+      <c r="L7">
+        <v>74349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>2024</v>
       </c>
       <c r="B8">
-        <v>9425497.51</v>
+        <v>8510815.33</v>
       </c>
       <c r="C8">
-        <v>35.95445578330019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1052835.53</v>
+      </c>
+      <c r="D8">
+        <v>9563650.859999999</v>
+      </c>
+      <c r="E8">
+        <v>11.00871984362675</v>
+      </c>
+      <c r="F8">
+        <v>88.99128015637326</v>
+      </c>
+      <c r="G8">
+        <v>-12.12502300922944</v>
+      </c>
+      <c r="H8">
+        <v>42.75354996247837</v>
+      </c>
+      <c r="I8">
+        <v>33.57053937951158</v>
+      </c>
+      <c r="J8">
+        <v>73484</v>
+      </c>
+      <c r="K8">
+        <v>3279</v>
+      </c>
+      <c r="L8">
+        <v>76763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>3265484.16</v>
+        <v>3098380.93</v>
       </c>
       <c r="C9">
-        <v>-65.35478199919443</v>
+        <v>322046.99</v>
+      </c>
+      <c r="D9">
+        <v>3420427.92</v>
+      </c>
+      <c r="E9">
+        <v>9.415400573621795</v>
+      </c>
+      <c r="F9">
+        <v>90.5845994263782</v>
+      </c>
+      <c r="G9">
+        <v>-69.4114625861838</v>
+      </c>
+      <c r="H9">
+        <v>-63.59478134746463</v>
+      </c>
+      <c r="I9">
+        <v>-64.23512348923201</v>
+      </c>
+      <c r="J9">
+        <v>22866</v>
+      </c>
+      <c r="K9">
+        <v>908</v>
+      </c>
+      <c r="L9">
+        <v>23774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizei analise de venda mensal por loja e faturamento diario
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -713,37 +713,37 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>3098380.93</v>
+        <v>3119447.96</v>
       </c>
       <c r="C9">
-        <v>322046.99</v>
+        <v>324756.99</v>
       </c>
       <c r="D9">
-        <v>3420427.92</v>
+        <v>3444204.95</v>
       </c>
       <c r="E9">
-        <v>9.415400573621795</v>
+        <v>9.429084352253774</v>
       </c>
       <c r="F9">
-        <v>90.5845994263782</v>
+        <v>90.57091564774622</v>
       </c>
       <c r="G9">
-        <v>-69.4114625861838</v>
+        <v>-69.15406245835948</v>
       </c>
       <c r="H9">
-        <v>-63.59478134746463</v>
+        <v>-63.34724889395527</v>
       </c>
       <c r="I9">
-        <v>-64.23512348923201</v>
+        <v>-63.98650473110224</v>
       </c>
       <c r="J9">
-        <v>22866</v>
+        <v>23100</v>
       </c>
       <c r="K9">
-        <v>908</v>
+        <v>918</v>
       </c>
       <c r="L9">
-        <v>23774</v>
+        <v>24018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao dos dados da bibi
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -713,37 +713,37 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>2535792.38</v>
+        <v>2554225.24</v>
       </c>
       <c r="C9">
-        <v>360196.99</v>
+        <v>368296.99</v>
       </c>
       <c r="D9">
-        <v>2895989.37</v>
+        <v>2922522.23</v>
       </c>
       <c r="E9">
-        <v>12.43778702129697</v>
+        <v>12.60202527184883</v>
       </c>
       <c r="F9">
-        <v>87.56221297870302</v>
+        <v>87.39797472815115</v>
       </c>
       <c r="G9">
-        <v>-65.18875694149187</v>
+        <v>-64.40593232995384</v>
       </c>
       <c r="H9">
-        <v>-54.20709468988187</v>
+        <v>-53.87422271691116</v>
       </c>
       <c r="I9">
-        <v>-55.9360167678435</v>
+        <v>-55.53230551453142</v>
       </c>
       <c r="J9">
-        <v>25089</v>
+        <v>25323</v>
       </c>
       <c r="K9">
-        <v>1042</v>
+        <v>1061</v>
       </c>
       <c r="L9">
-        <v>26131</v>
+        <v>26384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizando para visitar clientes - by matheus
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -713,37 +713,37 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>2589270.31</v>
+        <v>2646143.56</v>
       </c>
       <c r="C9">
-        <v>369816.99</v>
+        <v>401026.99</v>
       </c>
       <c r="D9">
-        <v>2959087.3</v>
+        <v>3047170.55</v>
       </c>
       <c r="E9">
-        <v>12.49767081897178</v>
+        <v>13.16063487158604</v>
       </c>
       <c r="F9">
-        <v>87.50232918102823</v>
+        <v>86.83936512841397</v>
       </c>
       <c r="G9">
-        <v>-64.25903190902325</v>
+        <v>-61.24274102925761</v>
       </c>
       <c r="H9">
-        <v>-53.24135719339522</v>
+        <v>-52.21430491085437</v>
       </c>
       <c r="I9">
-        <v>-54.97594897260026</v>
+        <v>-53.63571654935976</v>
       </c>
       <c r="J9">
-        <v>25544</v>
+        <v>26309</v>
       </c>
       <c r="K9">
-        <v>1066</v>
+        <v>1120</v>
       </c>
       <c r="L9">
-        <v>26610</v>
+        <v>27429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao p apresentar p bibi
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -713,37 +713,37 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>2589270.31</v>
+        <v>2646143.56</v>
       </c>
       <c r="C9">
-        <v>369816.99</v>
+        <v>401026.99</v>
       </c>
       <c r="D9">
-        <v>2959087.3</v>
+        <v>3047170.55</v>
       </c>
       <c r="E9">
-        <v>12.49767081897178</v>
+        <v>13.16063487158604</v>
       </c>
       <c r="F9">
-        <v>87.50232918102823</v>
+        <v>86.83936512841397</v>
       </c>
       <c r="G9">
-        <v>-64.25903190902325</v>
+        <v>-61.24274102925761</v>
       </c>
       <c r="H9">
-        <v>-53.24135719339522</v>
+        <v>-52.21430491085437</v>
       </c>
       <c r="I9">
-        <v>-54.97594897260026</v>
+        <v>-53.63571654935976</v>
       </c>
       <c r="J9">
-        <v>25544</v>
+        <v>26309</v>
       </c>
       <c r="K9">
-        <v>1066</v>
+        <v>1120</v>
       </c>
       <c r="L9">
-        <v>26610</v>
+        <v>27429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizei dados da bibi e adicionei ean no resultado da modelagem de estoque
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_anual.xlsx
@@ -713,37 +713,37 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>2716561.69</v>
+        <v>2742947.48</v>
       </c>
       <c r="C9">
-        <v>416701.99</v>
+        <v>418881.99</v>
       </c>
       <c r="D9">
-        <v>3133263.68</v>
+        <v>3161829.47</v>
       </c>
       <c r="E9">
-        <v>13.29929532135642</v>
+        <v>13.24808924625527</v>
       </c>
       <c r="F9">
-        <v>86.70070467864358</v>
+        <v>86.75191075374474</v>
       </c>
       <c r="G9">
-        <v>-59.72783043841088</v>
+        <v>-59.517144308392</v>
       </c>
       <c r="H9">
-        <v>-50.94265081778324</v>
+        <v>-50.46615992186744</v>
       </c>
       <c r="I9">
-        <v>-52.32576483613096</v>
+        <v>-51.89112149640997</v>
       </c>
       <c r="J9">
-        <v>26997</v>
+        <v>27232</v>
       </c>
       <c r="K9">
-        <v>1149</v>
+        <v>1155</v>
       </c>
       <c r="L9">
-        <v>28146</v>
+        <v>28387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>